<commit_message>
add scenario,session and correct scripts and profile
</commit_message>
<xml_diff>
--- a/Документация/WebTours Профиль нагрузки_v1.1.xlsx
+++ b/Документация/WebTours Профиль нагрузки_v1.1.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="70">
   <si>
     <t>Вход в систему</t>
   </si>
@@ -225,6 +225,27 @@
   </si>
   <si>
     <t>Количество запросов одним пользователем в минуту</t>
+  </si>
+  <si>
+    <t>choose_flight</t>
+  </si>
+  <si>
+    <t>click_itinerary</t>
+  </si>
+  <si>
+    <t>delete_ticket</t>
+  </si>
+  <si>
+    <t>fill_payment</t>
+  </si>
+  <si>
+    <t>Gotosite</t>
+  </si>
+  <si>
+    <t>fill_find_flights/click_flights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                              100/99</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1057,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Администратор" refreshedDate="44094.612729629633" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="25">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Администратор" refreshedDate="44094.77139490741" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="25">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H26" sheet="Автоматизированный расчет"/>
   </cacheSource>
@@ -1698,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,6 +1872,10 @@
         <f>SUM(R2:R7)</f>
         <v>10</v>
       </c>
+      <c r="X2">
+        <f>R2*S2*T2</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1919,6 +1944,10 @@
         <f t="shared" ref="V3:V7" si="5">R3/W$2</f>
         <v>0.1</v>
       </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X7" si="6">R3*S3*T3</f>
+        <v>24.489795918367349</v>
+      </c>
     </row>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1987,6 +2016,10 @@
         <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
+      <c r="X4">
+        <f t="shared" si="6"/>
+        <v>43.636363636363633</v>
+      </c>
     </row>
     <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -2055,6 +2088,10 @@
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
+      <c r="X5">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -2123,6 +2160,10 @@
         <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
+      <c r="X6">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2191,6 +2232,10 @@
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
+      <c r="X7">
+        <f t="shared" si="6"/>
+        <v>17.142857142857142</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2464,7 +2509,7 @@
         <v>130.90909090909091</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -2492,7 +2537,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -2520,7 +2565,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2548,7 +2593,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2576,7 +2621,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2604,7 +2649,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2632,7 +2677,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2660,7 +2705,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -2688,7 +2733,7 @@
         <v>51.428571428571423</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2716,7 +2761,7 @@
         <v>51.428571428571423</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2744,7 +2789,7 @@
         <v>51.428571428571423</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
         <v>40</v>
       </c>
@@ -2754,8 +2799,14 @@
       <c r="G28" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K28" t="s">
+        <v>67</v>
+      </c>
+      <c r="L28">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2775,14 +2826,20 @@
         <v>140.26901669758811</v>
       </c>
       <c r="H29" s="33">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="I29" s="26">
         <f>1-G29/H29</f>
-        <v>7.7177521726394027E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>-1.9215478399150498E-3</v>
+      </c>
+      <c r="K29" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -2794,22 +2851,28 @@
         <v>299.33766233766232</v>
       </c>
       <c r="D30" s="26">
-        <f t="shared" ref="D30:D36" si="6">1-B30/C30</f>
+        <f t="shared" ref="D30:D36" si="7">1-B30/C30</f>
         <v>5.7920083300793901E-2</v>
       </c>
       <c r="G30" s="33">
-        <f t="shared" ref="G30:G35" si="7">C30/3</f>
+        <f t="shared" ref="G30:G35" si="8">C30/3</f>
         <v>99.779220779220779</v>
       </c>
       <c r="H30" s="33">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I30" s="26">
-        <f t="shared" ref="I30:I35" si="8">1-G30/H30</f>
-        <v>9.2916174734356538E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I30:I35" si="9">1-G30/H30</f>
+        <v>2.2077922077922141E-3</v>
+      </c>
+      <c r="K30" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -2821,22 +2884,28 @@
         <v>247.90909090909091</v>
       </c>
       <c r="D31" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.2467913458012569E-2</v>
       </c>
       <c r="G31" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>82.63636363636364</v>
       </c>
       <c r="H31" s="33">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I31" s="26">
-        <f t="shared" si="8"/>
-        <v>9.1908091908091905E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>-7.7605321507761005E-3</v>
+      </c>
+      <c r="K31" t="s">
+        <v>63</v>
+      </c>
+      <c r="L31">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -2848,22 +2917,28 @@
         <v>175.90909090909091</v>
       </c>
       <c r="D32" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.1679586563306845E-3</v>
       </c>
       <c r="G32" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>58.636363636363633</v>
       </c>
       <c r="H32" s="33">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I32" s="26">
-        <f t="shared" si="8"/>
-        <v>6.9264069264069361E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>-1.097178683385569E-2</v>
+      </c>
+      <c r="K32" t="s">
+        <v>66</v>
+      </c>
+      <c r="L32">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2875,22 +2950,28 @@
         <v>166.46938775510205</v>
       </c>
       <c r="D33" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.4869437293122538E-2</v>
       </c>
       <c r="G33" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>55.489795918367349</v>
       </c>
       <c r="H33" s="33">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I33" s="26">
-        <f t="shared" si="8"/>
-        <v>7.5170068027210823E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>9.1107871720116362E-3</v>
+      </c>
+      <c r="K33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L33">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -2901,22 +2982,28 @@
         <v>73</v>
       </c>
       <c r="D34" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G34" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24.333333333333332</v>
       </c>
       <c r="H34" s="33">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I34" s="26">
-        <f t="shared" si="8"/>
-        <v>9.8765432098765427E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>2.6666666666666727E-2</v>
+      </c>
+      <c r="K34" t="s">
+        <v>65</v>
+      </c>
+      <c r="L34">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -2928,22 +3015,28 @@
         <v>420.80705009276437</v>
       </c>
       <c r="D35" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.834909507748673E-3</v>
       </c>
       <c r="G35" s="33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>140.26901669758811</v>
       </c>
       <c r="H35" s="33">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="I35" s="26">
-        <f t="shared" si="8"/>
-        <v>7.1066114585509155E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>-9.1296165294108E-3</v>
+      </c>
+      <c r="K35" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2955,13 +3048,14 @@
         <v>1804.2393320964748</v>
       </c>
       <c r="D36" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.4425672375409304E-2</v>
       </c>
       <c r="E36" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add session and correct skript and scenario
</commit_message>
<xml_diff>
--- a/Документация/WebTours Профиль нагрузки_v1.1.xlsx
+++ b/Документация/WebTours Профиль нагрузки_v1.1.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="77">
   <si>
     <t>Вход в систему</t>
   </si>
@@ -245,10 +245,28 @@
     <t>fill_find_flights/click_flights</t>
   </si>
   <si>
-    <t xml:space="preserve">                                              100/99</t>
-  </si>
-  <si>
     <t>t=[0,32: 20,32]</t>
+  </si>
+  <si>
+    <t>отладочный тест</t>
+  </si>
+  <si>
+    <t>тест поиска максимума</t>
+  </si>
+  <si>
+    <t>400/399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    100/99</t>
+  </si>
+  <si>
+    <t>t=[1:09:34, 1:29:34]</t>
+  </si>
+  <si>
+    <t>тест подтверждения максимума</t>
+  </si>
+  <si>
+    <t>операц/час</t>
   </si>
 </sst>
 </file>
@@ -478,7 +496,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -679,6 +697,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,7 +950,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -995,6 +1025,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="38" borderId="0" xfId="44" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1720,23 +1753,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X36"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="K21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="44" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" customWidth="1"/>
     <col min="21" max="21" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2512,7 +2546,7 @@
         <v>130.90909090909091</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -2540,7 +2574,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -2568,7 +2602,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2596,7 +2630,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2624,7 +2658,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2652,7 +2686,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2680,7 +2714,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2708,7 +2742,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -2736,7 +2770,7 @@
         <v>51.428571428571423</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2764,7 +2798,7 @@
         <v>51.428571428571423</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2792,12 +2826,15 @@
         <v>51.428571428571423</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="R27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
         <v>40</v>
       </c>
@@ -2807,14 +2844,41 @@
       <c r="G28" t="s">
         <v>56</v>
       </c>
-      <c r="K28" t="s">
+      <c r="I28" t="s">
+        <v>70</v>
+      </c>
+      <c r="K28" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="40">
         <v>141</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
+        <v>56</v>
+      </c>
+      <c r="P28" t="s">
+        <v>71</v>
+      </c>
+      <c r="R28" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="S28" s="40">
+        <v>559</v>
+      </c>
+      <c r="U28" t="s">
+        <v>56</v>
+      </c>
+      <c r="W28" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y28" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z28" s="40">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2836,18 +2900,52 @@
       <c r="H29" s="33">
         <v>140</v>
       </c>
-      <c r="I29" s="26">
+      <c r="I29" s="39">
         <f>1-G29/H29</f>
         <v>-1.9215478399150498E-3</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="40">
         <v>140</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N29" s="33">
+        <f>C29/3*4</f>
+        <v>561.07606679035246</v>
+      </c>
+      <c r="O29" s="33">
+        <v>561</v>
+      </c>
+      <c r="P29" s="39">
+        <f>1-N29/O29</f>
+        <v>-1.3559142665320323E-4</v>
+      </c>
+      <c r="R29" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="S29" s="40">
+        <v>561</v>
+      </c>
+      <c r="U29" s="33">
+        <f>C29*4</f>
+        <v>1683.2282003710575</v>
+      </c>
+      <c r="V29" s="33">
+        <v>1684</v>
+      </c>
+      <c r="W29" s="39">
+        <f>1-U29/V29</f>
+        <v>4.5831331884949034E-4</v>
+      </c>
+      <c r="Y29" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z29" s="40">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
@@ -2859,28 +2957,62 @@
         <v>299.33766233766232</v>
       </c>
       <c r="D30" s="26">
-        <f t="shared" ref="D30:D36" si="7">1-B30/C30</f>
+        <f>1-B30/C30</f>
         <v>5.7920083300793901E-2</v>
       </c>
       <c r="G30" s="33">
-        <f t="shared" ref="G30:G35" si="8">C30/3</f>
+        <f t="shared" ref="G30:G35" si="7">C30/3</f>
         <v>99.779220779220779</v>
       </c>
       <c r="H30" s="33">
         <v>100</v>
       </c>
-      <c r="I30" s="26">
-        <f t="shared" ref="I30:I35" si="9">1-G30/H30</f>
+      <c r="I30" s="39">
+        <f t="shared" ref="I30:I35" si="8">1-G30/H30</f>
         <v>2.2077922077922141E-3</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="L30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L30" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="N30" s="33">
+        <f t="shared" ref="N30:N35" si="9">C30/3*4</f>
+        <v>399.11688311688312</v>
+      </c>
+      <c r="O30" s="33">
+        <v>400</v>
+      </c>
+      <c r="P30" s="39">
+        <f t="shared" ref="P30:P35" si="10">1-N30/O30</f>
+        <v>2.2077922077922141E-3</v>
+      </c>
+      <c r="R30" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="S30" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="U30" s="33">
+        <f t="shared" ref="U30:U35" si="11">C30*4</f>
+        <v>1197.3506493506493</v>
+      </c>
+      <c r="V30" s="33">
+        <v>1197</v>
+      </c>
+      <c r="W30" s="39">
+        <f t="shared" ref="W30:W35" si="12">1-U30/V30</f>
+        <v>-2.9294014256420198E-4</v>
+      </c>
+      <c r="Y30" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z30" s="40">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -2892,28 +3024,62 @@
         <v>247.90909090909091</v>
       </c>
       <c r="D31" s="26">
+        <f t="shared" ref="D31:D36" si="13">1-B31/C31</f>
+        <v>-1.2467913458012569E-2</v>
+      </c>
+      <c r="G31" s="33">
         <f t="shared" si="7"/>
-        <v>-1.2467913458012569E-2</v>
-      </c>
-      <c r="G31" s="33">
-        <f t="shared" si="8"/>
         <v>82.63636363636364</v>
       </c>
       <c r="H31" s="33">
         <v>82</v>
       </c>
-      <c r="I31" s="26">
+      <c r="I31" s="39">
+        <f t="shared" si="8"/>
+        <v>-7.7605321507761005E-3</v>
+      </c>
+      <c r="K31" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="L31" s="40">
+        <v>82</v>
+      </c>
+      <c r="N31" s="33">
         <f t="shared" si="9"/>
-        <v>-7.7605321507761005E-3</v>
-      </c>
-      <c r="K31" t="s">
+        <v>330.54545454545456</v>
+      </c>
+      <c r="O31" s="33">
+        <v>331</v>
+      </c>
+      <c r="P31" s="39">
+        <f t="shared" si="10"/>
+        <v>1.3732491073880082E-3</v>
+      </c>
+      <c r="R31" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="L31">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S31" s="40">
+        <v>331</v>
+      </c>
+      <c r="U31" s="33">
+        <f t="shared" si="11"/>
+        <v>991.63636363636363</v>
+      </c>
+      <c r="V31" s="33">
+        <v>991</v>
+      </c>
+      <c r="W31" s="39">
+        <f t="shared" si="12"/>
+        <v>-6.4214292266773221E-4</v>
+      </c>
+      <c r="Y31" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z31" s="40">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -2925,28 +3091,62 @@
         <v>175.90909090909091</v>
       </c>
       <c r="D32" s="26">
+        <f t="shared" si="13"/>
+        <v>5.1679586563306845E-3</v>
+      </c>
+      <c r="G32" s="33">
         <f t="shared" si="7"/>
-        <v>5.1679586563306845E-3</v>
-      </c>
-      <c r="G32" s="33">
-        <f t="shared" si="8"/>
         <v>58.636363636363633</v>
       </c>
       <c r="H32" s="33">
         <v>59</v>
       </c>
-      <c r="I32" s="26">
+      <c r="I32" s="39">
+        <f t="shared" si="8"/>
+        <v>6.1633281972265364E-3</v>
+      </c>
+      <c r="K32" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="L32" s="40">
+        <v>59</v>
+      </c>
+      <c r="N32" s="33">
         <f t="shared" si="9"/>
-        <v>6.1633281972265364E-3</v>
-      </c>
-      <c r="K32" t="s">
+        <v>234.54545454545453</v>
+      </c>
+      <c r="O32" s="33">
+        <v>235</v>
+      </c>
+      <c r="P32" s="39">
+        <f t="shared" si="10"/>
+        <v>1.9342359767892114E-3</v>
+      </c>
+      <c r="R32" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="L32">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S32" s="40">
+        <v>235</v>
+      </c>
+      <c r="U32" s="33">
+        <f t="shared" si="11"/>
+        <v>703.63636363636363</v>
+      </c>
+      <c r="V32" s="33">
+        <v>704</v>
+      </c>
+      <c r="W32" s="39">
+        <f t="shared" si="12"/>
+        <v>5.1652892561981911E-4</v>
+      </c>
+      <c r="Y32" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z32" s="40">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2958,28 +3158,62 @@
         <v>166.46938775510205</v>
       </c>
       <c r="D33" s="26">
+        <f t="shared" si="13"/>
+        <v>4.4869437293122538E-2</v>
+      </c>
+      <c r="G33" s="33">
         <f t="shared" si="7"/>
-        <v>4.4869437293122538E-2</v>
-      </c>
-      <c r="G33" s="33">
-        <f t="shared" si="8"/>
         <v>55.489795918367349</v>
       </c>
       <c r="H33" s="33">
         <v>56</v>
       </c>
-      <c r="I33" s="26">
+      <c r="I33" s="39">
+        <f t="shared" si="8"/>
+        <v>9.1107871720116362E-3</v>
+      </c>
+      <c r="K33" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="L33" s="40">
+        <v>56</v>
+      </c>
+      <c r="N33" s="33">
         <f t="shared" si="9"/>
-        <v>9.1107871720116362E-3</v>
-      </c>
-      <c r="K33" t="s">
+        <v>221.9591836734694</v>
+      </c>
+      <c r="O33" s="33">
+        <v>223</v>
+      </c>
+      <c r="P33" s="39">
+        <f t="shared" si="10"/>
+        <v>4.667337787132797E-3</v>
+      </c>
+      <c r="R33" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="L33">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S33" s="40">
+        <v>223</v>
+      </c>
+      <c r="U33" s="33">
+        <f t="shared" si="11"/>
+        <v>665.87755102040819</v>
+      </c>
+      <c r="V33" s="33">
+        <v>668</v>
+      </c>
+      <c r="W33" s="39">
+        <f t="shared" si="12"/>
+        <v>3.1773188317242296E-3</v>
+      </c>
+      <c r="Y33" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z33" s="40">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -2990,28 +3224,62 @@
         <v>73</v>
       </c>
       <c r="D34" s="26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="33">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="33">
-        <f t="shared" si="8"/>
         <v>24.333333333333332</v>
       </c>
       <c r="H34" s="33">
         <v>25</v>
       </c>
-      <c r="I34" s="26">
+      <c r="I34" s="39">
+        <f t="shared" si="8"/>
+        <v>2.6666666666666727E-2</v>
+      </c>
+      <c r="K34" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="L34" s="40">
+        <v>25</v>
+      </c>
+      <c r="N34" s="33">
         <f t="shared" si="9"/>
+        <v>97.333333333333329</v>
+      </c>
+      <c r="O34" s="33">
+        <v>100</v>
+      </c>
+      <c r="P34" s="39">
+        <f t="shared" si="10"/>
         <v>2.6666666666666727E-2</v>
       </c>
-      <c r="K34" t="s">
+      <c r="R34" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="L34">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S34" s="40">
+        <v>100</v>
+      </c>
+      <c r="U34" s="33">
+        <f t="shared" si="11"/>
+        <v>292</v>
+      </c>
+      <c r="V34" s="33">
+        <v>295</v>
+      </c>
+      <c r="W34" s="39">
+        <f t="shared" si="12"/>
+        <v>1.016949152542368E-2</v>
+      </c>
+      <c r="Y34" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z34" s="40">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -3023,28 +3291,62 @@
         <v>420.80705009276437</v>
       </c>
       <c r="D35" s="26">
+        <f t="shared" si="13"/>
+        <v>-2.834909507748673E-3</v>
+      </c>
+      <c r="G35" s="33">
         <f t="shared" si="7"/>
-        <v>-2.834909507748673E-3</v>
-      </c>
-      <c r="G35" s="33">
-        <f t="shared" si="8"/>
         <v>140.26901669758811</v>
       </c>
       <c r="H35" s="33">
         <v>141</v>
       </c>
-      <c r="I35" s="26">
+      <c r="I35" s="39">
+        <f t="shared" si="8"/>
+        <v>5.1842787405098623E-3</v>
+      </c>
+      <c r="K35" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35" s="40">
+        <v>141</v>
+      </c>
+      <c r="N35" s="33">
         <f t="shared" si="9"/>
-        <v>5.1842787405098623E-3</v>
-      </c>
-      <c r="K35" t="s">
+        <v>561.07606679035246</v>
+      </c>
+      <c r="O35" s="33">
+        <v>562</v>
+      </c>
+      <c r="P35" s="39">
+        <f t="shared" si="10"/>
+        <v>1.6440092698354336E-3</v>
+      </c>
+      <c r="R35" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="L35">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S35" s="40">
+        <v>562</v>
+      </c>
+      <c r="U35" s="33">
+        <f t="shared" si="11"/>
+        <v>1683.2282003710575</v>
+      </c>
+      <c r="V35" s="33">
+        <v>1683</v>
+      </c>
+      <c r="W35" s="39">
+        <f t="shared" si="12"/>
+        <v>-1.3559142665320323E-4</v>
+      </c>
+      <c r="Y35" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z35" s="40">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -3056,10 +3358,17 @@
         <v>1804.2393320964748</v>
       </c>
       <c r="D36" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>6.4425672375409304E-2</v>
       </c>
       <c r="E36" s="4"/>
+      <c r="O36">
+        <f>SUM(O29:O35)*3</f>
+        <v>7236</v>
+      </c>
+      <c r="P36" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3094,13 +3403,13 @@
   </cols>
   <sheetData>
     <row r="9" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="11" spans="5:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="E11" s="5" t="s">
@@ -3253,13 +3562,13 @@
       </c>
     </row>
     <row r="23" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
     </row>
     <row r="25" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E25" s="12" t="s">
@@ -3419,13 +3728,13 @@
       </c>
     </row>
     <row r="35" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E35" s="38" t="s">
+      <c r="E35" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
     </row>
     <row r="37" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E37" s="12" t="s">

</xml_diff>

<commit_message>
add sessions and otchet
</commit_message>
<xml_diff>
--- a/Документация/WebTours Профиль нагрузки_v1.1.xlsx
+++ b/Документация/WebTours Профиль нагрузки_v1.1.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="76">
   <si>
     <t>Вход в систему</t>
   </si>
@@ -254,9 +254,6 @@
     <t>тест поиска максимума</t>
   </si>
   <si>
-    <t>400/399</t>
-  </si>
-  <si>
     <t xml:space="preserve">    100/99</t>
   </si>
   <si>
@@ -266,7 +263,7 @@
     <t>тест подтверждения максимума</t>
   </si>
   <si>
-    <t>операц/час</t>
+    <t>запросов/час</t>
   </si>
 </sst>
 </file>
@@ -1755,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="K24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,7 +2828,7 @@
         <v>69</v>
       </c>
       <c r="R27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
@@ -2869,7 +2866,7 @@
         <v>56</v>
       </c>
       <c r="W28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Y28" s="38" t="s">
         <v>67</v>
@@ -2975,24 +2972,24 @@
         <v>68</v>
       </c>
       <c r="L30" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N30" s="33">
         <f t="shared" ref="N30:N35" si="9">C30/3*4</f>
         <v>399.11688311688312</v>
       </c>
       <c r="O30" s="33">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P30" s="39">
         <f t="shared" ref="P30:P35" si="10">1-N30/O30</f>
-        <v>2.2077922077922141E-3</v>
+        <v>-2.9294014256420198E-4</v>
       </c>
       <c r="R30" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="S30" s="40" t="s">
-        <v>72</v>
+      <c r="S30" s="40">
+        <v>399</v>
       </c>
       <c r="U30" s="33">
         <f t="shared" ref="U30:U35" si="11">C30*4</f>
@@ -3116,17 +3113,17 @@
         <v>234.54545454545453</v>
       </c>
       <c r="O32" s="33">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="P32" s="39">
         <f t="shared" si="10"/>
-        <v>1.9342359767892114E-3</v>
+        <v>6.1633281972265364E-3</v>
       </c>
       <c r="R32" s="38" t="s">
         <v>66</v>
       </c>
       <c r="S32" s="40">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="U32" s="33">
         <f t="shared" si="11"/>
@@ -3367,7 +3364,14 @@
         <v>7236</v>
       </c>
       <c r="P36" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="V36">
+        <f>SUM(V29:V35)</f>
+        <v>7222</v>
+      </c>
+      <c r="W36" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>